<commit_message>
ignoring your excel modifications done by you OS
</commit_message>
<xml_diff>
--- a/Mini Project Agile Plan.xlsx
+++ b/Mini Project Agile Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\City-Guesser-CS2-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F337545-79EF-40C0-8CC9-5CE923683951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FA581B-E680-42FC-8889-F327EE4BA600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7606A27B-A156-4B35-AD7A-2919D948A378}"/>
+    <workbookView xWindow="-25380" yWindow="3390" windowWidth="21600" windowHeight="11295" xr2:uid="{7606A27B-A156-4B35-AD7A-2919D948A378}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Day</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>DONE: used springboot, got a second API</t>
+  </si>
+  <si>
+    <t>REWORKED</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,6 +527,9 @@
       <c r="G6" t="s">
         <v>6</v>
       </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -532,8 +538,14 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="I8" t="s">
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
         <v>10</v>
+      </c>
+      <c r="P8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Mini Project Agile Plan.xlsx
</commit_message>
<xml_diff>
--- a/Mini Project Agile Plan.xlsx
+++ b/Mini Project Agile Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\City-Guesser-CS2-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FA581B-E680-42FC-8889-F327EE4BA600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FA4B28-30F6-47BF-B3E0-09C91C82D59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25380" yWindow="3390" windowWidth="21600" windowHeight="11295" xr2:uid="{7606A27B-A156-4B35-AD7A-2919D948A378}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Day</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>REWORKED</t>
+  </si>
+  <si>
+    <t>MINIMAL</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +566,9 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -573,6 +579,9 @@
       </c>
       <c r="G14" t="s">
         <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>